<commit_message>
Updated concentration calculations. Added a script to generate combination stock plate layouts.
</commit_message>
<xml_diff>
--- a/Drafts/Stressor Concentration Calculations.xlsx
+++ b/Drafts/Stressor Concentration Calculations.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Welch\Google Drive\ICL Ecological Applications\Project\Work\Drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF0A19F-823D-4E71-80DD-2C18D3FBBF5F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC61532-3327-4E35-9978-DEEBC43D77F1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="2" xr2:uid="{5489DA95-FB90-4042-A69A-9A87661BC295}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="1" xr2:uid="{5489DA95-FB90-4042-A69A-9A87661BC295}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentration Calculator" sheetId="2" r:id="rId1"/>
     <sheet name="IStock Plate 1" sheetId="1" r:id="rId2"/>
-    <sheet name="IStock Plate 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
   <si>
     <t>Chloramphenicol</t>
   </si>
@@ -83,9 +82,6 @@
     <t>Required Indiv Stock Volume (L)</t>
   </si>
   <si>
-    <t xml:space="preserve">= 127 * CSV </t>
-  </si>
-  <si>
     <t>Will flag if any indiv stock concentrations are close to solubility limits</t>
   </si>
   <si>
@@ -95,9 +91,6 @@
     <t>NiCl2</t>
   </si>
   <si>
-    <t>75.7 g/100 mL</t>
-  </si>
-  <si>
     <t>Solubility at ~room temperature (mg/L)</t>
   </si>
   <si>
@@ -119,7 +112,10 @@
     <t>Benz</t>
   </si>
   <si>
-    <t>You need one of these and one of Plate 2 for every isolate you're using</t>
+    <t>2mL all</t>
+  </si>
+  <si>
+    <t>= 127 * CSV * 0.5</t>
   </si>
 </sst>
 </file>
@@ -168,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +187,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -210,6 +215,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,7 +557,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,10 +577,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -726,46 +740,46 @@
         <v>17</v>
       </c>
       <c r="B8" s="7">
-        <f>127*$P$5</f>
-        <v>3.175E-2</v>
+        <f>127*$P$5*0.5</f>
+        <v>1.5875E-2</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" ref="C8:I8" si="2">127*$P$5</f>
-        <v>3.175E-2</v>
+        <f t="shared" ref="C8:I8" si="2">127*$P$5*0.5</f>
+        <v>1.5875E-2</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="2"/>
-        <v>3.175E-2</v>
+        <v>1.5875E-2</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="2"/>
-        <v>3.175E-2</v>
+        <v>1.5875E-2</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="2"/>
-        <v>3.175E-2</v>
+        <v>1.5875E-2</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="2"/>
-        <v>3.175E-2</v>
+        <v>1.5875E-2</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" si="2"/>
-        <v>3.175E-2</v>
+        <v>1.5875E-2</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="2"/>
-        <v>3.175E-2</v>
+        <v>1.5875E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4">
         <v>757000</v>
@@ -794,13 +808,11 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D16" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -821,208 +833,228 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9617475C-EE97-49EB-AC49-215D642643BB}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="A1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
     <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>25</v>
+      <c r="A5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>26</v>
+      <c r="A8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1031,64 +1063,28 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1102,283 +1098,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF8EB60-E0EE-4314-8168-30B01AF999DF}">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>